<commit_message>
Update data processing logic and requirements.txt for machine learning model training.
</commit_message>
<xml_diff>
--- a/Data/ONI/ONI_historico.xlsx
+++ b/Data/ONI/ONI_historico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Documentos\Personal\Repos\JSSL-INV-FUNC-BACKEND\Data\ONI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D4C013-4F87-4238-B78C-11D42EA507D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F22501-8915-48A6-B7D8-99CA3198D375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>ONI</t>
+    <t>ANOM</t>
   </si>
   <si>
-    <t>ANOM</t>
+    <t>SST</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C904"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,10 +413,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>